<commit_message>
updated training result log
</commit_message>
<xml_diff>
--- a/Assessment/Projects/Final Project/src/trainingData/result.xlsx
+++ b/Assessment/Projects/Final Project/src/trainingData/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dylim/Documents/CASA/CE/casa0018/Assessment/Projects/Final Project/src/trainingData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626DA21A-8D13-7B40-A6EE-9C3FF2BA6842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD12A1C9-16AB-3045-8CAA-F24ADC184BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{2CAA837F-BAC6-CB46-8215-D6147D7E7B28}"/>
+    <workbookView xWindow="5180" yWindow="660" windowWidth="28040" windowHeight="17440" xr2:uid="{2CAA837F-BAC6-CB46-8215-D6147D7E7B28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -478,7 +478,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>